<commit_message>
Minor fixes to the NUT16. It runs Hello World now!
</commit_message>
<xml_diff>
--- a/Architecture/NUT16 Instruction set.xlsx
+++ b/Architecture/NUT16 Instruction set.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukan\Desktop\cpp_dev\Custom Computer and Programing Language\Architecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE6DE90B-B573-4D72-B295-CEF3B1E2ACA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94727E86-B0DF-4BD6-A15D-E1310066EBA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47745" yWindow="0" windowWidth="9855" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v1.0" sheetId="3" r:id="rId1"/>
@@ -1176,8 +1176,8 @@
   <dimension ref="A1:Y55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2342,7 +2342,7 @@
         <v>0</v>
       </c>
       <c r="S17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="2">
         <v>0</v>
@@ -2358,11 +2358,11 @@
       </c>
       <c r="X17" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y17" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -2419,7 +2419,7 @@
         <v>0</v>
       </c>
       <c r="S18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="2">
         <v>0</v>
@@ -2435,11 +2435,11 @@
       </c>
       <c r="X18" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y18" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -2496,7 +2496,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="2">
         <v>0</v>
@@ -2512,11 +2512,11 @@
       </c>
       <c r="X19" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y19" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -2573,7 +2573,7 @@
         <v>0</v>
       </c>
       <c r="S20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20" s="2">
         <v>0</v>
@@ -2589,11 +2589,11 @@
       </c>
       <c r="X20" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y20" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -2650,7 +2650,7 @@
         <v>0</v>
       </c>
       <c r="S21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T21" s="2">
         <v>0</v>
@@ -2666,11 +2666,11 @@
       </c>
       <c r="X21" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y21" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
@@ -2727,7 +2727,7 @@
         <v>0</v>
       </c>
       <c r="S22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T22" s="2">
         <v>0</v>
@@ -2743,11 +2743,11 @@
       </c>
       <c r="X22" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y22" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
@@ -2804,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="S23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23" s="2">
         <v>0</v>
@@ -2820,11 +2820,11 @@
       </c>
       <c r="X23" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y23" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
@@ -2881,7 +2881,7 @@
         <v>0</v>
       </c>
       <c r="S24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" s="2">
         <v>0</v>
@@ -2897,11 +2897,11 @@
       </c>
       <c r="X24" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y24" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
@@ -2958,7 +2958,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" s="2">
         <v>0</v>
@@ -2974,11 +2974,11 @@
       </c>
       <c r="X25" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y25" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
@@ -3035,7 +3035,7 @@
         <v>0</v>
       </c>
       <c r="S26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="2">
         <v>0</v>
@@ -3051,11 +3051,11 @@
       </c>
       <c r="X26" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y26" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
@@ -3112,7 +3112,7 @@
         <v>0</v>
       </c>
       <c r="S27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T27" s="2">
         <v>0</v>
@@ -3128,11 +3128,11 @@
       </c>
       <c r="X27" s="13">
         <f t="shared" si="2"/>
-        <v>512</v>
+        <v>528</v>
       </c>
       <c r="Y27" s="13" t="str">
         <f t="shared" si="1"/>
-        <v>0200</v>
+        <v>0210</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>